<commit_message>
KPI for csm, rd, designer
</commit_message>
<xml_diff>
--- a/exports/KPI_Result_2025_7.xlsx
+++ b/exports/KPI_Result_2025_7.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,9 @@
       <c r="E1" t="str">
         <v>Target</v>
       </c>
+      <c r="F1" t="str">
+        <v>KPI</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -430,10 +433,13 @@
         <v>R&amp;D</v>
       </c>
       <c r="D2">
-        <v>687.87</v>
+        <v>488.74</v>
       </c>
       <c r="E2">
         <v>1417.14</v>
+      </c>
+      <c r="F2" t="str">
+        <v>34.49%</v>
       </c>
     </row>
     <row r="3">
@@ -447,10 +453,13 @@
         <v>Designer</v>
       </c>
       <c r="D3">
-        <v>47.37</v>
+        <v>1113.05</v>
       </c>
       <c r="E3">
         <v>3266.71</v>
+      </c>
+      <c r="F3" t="str">
+        <v>34.07%</v>
       </c>
     </row>
     <row r="4">
@@ -464,10 +473,13 @@
         <v>R&amp;D</v>
       </c>
       <c r="D4">
-        <v>29.59</v>
+        <v>-3.59</v>
       </c>
       <c r="E4">
         <v>1267.95</v>
+      </c>
+      <c r="F4" t="str">
+        <v>-0.28%</v>
       </c>
     </row>
     <row r="5">
@@ -481,10 +493,13 @@
         <v>R&amp;D</v>
       </c>
       <c r="D5">
-        <v>0.9</v>
+        <v>559.9</v>
       </c>
       <c r="E5">
         <v>1267.95</v>
+      </c>
+      <c r="F5" t="str">
+        <v>44.16%</v>
       </c>
     </row>
     <row r="6">
@@ -498,49 +513,98 @@
         <v>R&amp;D</v>
       </c>
       <c r="D6">
-        <v>0.9</v>
+        <v>39.37</v>
       </c>
       <c r="E6">
         <v>1267.95</v>
       </c>
+      <c r="F6" t="str">
+        <v>3.11%</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Thành  (BX)</v>
+        <v>Nhung (NU)</v>
       </c>
       <c r="B7" t="str">
-        <v>BX</v>
+        <v>NU</v>
       </c>
       <c r="C7" t="str">
-        <v>R&amp;D</v>
+        <v>CSM - Bán hàng</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5225.64</v>
       </c>
       <c r="E7">
-        <v>1899.48</v>
+        <v>5628.8</v>
+      </c>
+      <c r="F7" t="str">
+        <v>92.84%</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>Thiên Hà (HV)</v>
+      </c>
+      <c r="B8" t="str">
+        <v>HV</v>
+      </c>
+      <c r="C8" t="str">
+        <v>CSM - Bán hàng</v>
+      </c>
+      <c r="D8">
+        <v>5225.64</v>
+      </c>
+      <c r="E8">
+        <v>5628.8</v>
+      </c>
+      <c r="F8" t="str">
+        <v>92.84%</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Thành  (BX)</v>
+      </c>
+      <c r="B9" t="str">
+        <v>BX</v>
+      </c>
+      <c r="C9" t="str">
+        <v>R&amp;D</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1899.48</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0.00%</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Truong (XT)</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B10" t="str">
         <v>XT</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C10" t="str">
         <v>Designer</v>
       </c>
-      <c r="D8">
-        <v>0.9</v>
-      </c>
-      <c r="E8">
+      <c r="D10">
+        <v>2748.07</v>
+      </c>
+      <c r="E10">
         <v>3769.29</v>
+      </c>
+      <c r="F10" t="str">
+        <v>72.91%</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>